<commit_message>
retrained models, updated predictions
</commit_message>
<xml_diff>
--- a/GBM Lifetime Predictions.xlsx
+++ b/GBM Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FE1BB0-2B46-4855-9D30-1626EE23B8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21B8B71-8071-49D5-8D49-13505A39C364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>Playing At:  Seattle Kraken   Home</t>
+  </si>
+  <si>
+    <t>GBM2</t>
+  </si>
+  <si>
+    <t>80-85</t>
+  </si>
+  <si>
+    <t>70-80</t>
   </si>
 </sst>
 </file>
@@ -878,31 +887,32 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45290.441500231478" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{827BC2B5-8CB2-43F7-9795-87FC66DF261C}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45291.357700694447" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="60" xr:uid="{827BC2B5-8CB2-43F7-9795-87FC66DF261C}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A42:I1000" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Model Used" numFmtId="0">
-      <sharedItems containsBlank="1" count="2">
+      <sharedItems containsBlank="1" count="3">
         <s v="GBM1"/>
+        <s v="GBM2"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-23T00:00:00" maxDate="2023-12-31T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-23T00:00:00" maxDate="2024-01-01T00:00:00"/>
     </cacheField>
     <cacheField name="Winner" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.50199000000000005" maxValue="0.68823000000000001"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.50199000000000005" maxValue="0.80030000000000001"/>
     </cacheField>
     <cacheField name="Loser" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Loser Probability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.31176999999999999" maxValue="0.49801000000000001"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.19969999999999999" maxValue="0.49801000000000001"/>
     </cacheField>
     <cacheField name="Site" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -911,9 +921,11 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
+      <sharedItems containsBlank="1" count="5">
         <s v="60-70"/>
         <s v="50-60"/>
+        <s v="80-85"/>
+        <s v="70-80"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -928,7 +940,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="51">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
   <r>
     <x v="0"/>
     <d v="2023-12-23T00:00:00"/>
@@ -1388,7 +1400,7 @@
     <s v="New Jersey Devils"/>
     <n v="0.32350000000000001"/>
     <s v="Playing At:  Boston Bruins   Home"/>
-    <m/>
+    <n v="1"/>
     <x v="0"/>
   </r>
   <r>
@@ -1399,7 +1411,7 @@
     <s v="Montreal Canadiens"/>
     <n v="0.32940000000000003"/>
     <s v="Playing At:  Florida Panthers   Home"/>
-    <m/>
+    <n v="1"/>
     <x v="0"/>
   </r>
   <r>
@@ -1410,7 +1422,7 @@
     <s v="Minnesota Wild"/>
     <n v="0.38009999999999999"/>
     <s v="Playing At:  Winnipeg Jets   Home"/>
-    <m/>
+    <n v="1"/>
     <x v="0"/>
   </r>
   <r>
@@ -1421,7 +1433,7 @@
     <s v="Edmonton Oilers"/>
     <n v="0.38419999999999999"/>
     <s v="Playing At:  Los Angeles Kings   Home"/>
-    <m/>
+    <n v="0"/>
     <x v="0"/>
   </r>
   <r>
@@ -1432,7 +1444,7 @@
     <s v="Columbus Blue Jackets"/>
     <n v="0.4073"/>
     <s v="Playing At:  Buffalo Sabres   Home"/>
-    <m/>
+    <n v="1"/>
     <x v="1"/>
   </r>
   <r>
@@ -1443,7 +1455,7 @@
     <s v="New York Rangers"/>
     <n v="0.41760000000000003"/>
     <s v="Playing At:  Tampa Bay Lightning   Home"/>
-    <m/>
+    <n v="0"/>
     <x v="1"/>
   </r>
   <r>
@@ -1454,7 +1466,7 @@
     <s v="Carolina Hurricanes"/>
     <n v="0.45229999999999998"/>
     <s v="Playing At:  Toronto Maple Leafs   Home"/>
-    <m/>
+    <n v="0"/>
     <x v="1"/>
   </r>
   <r>
@@ -1465,7 +1477,7 @@
     <s v="Washington Capitals"/>
     <n v="0.46679999999999999"/>
     <s v="Playing At:  Washington Capitals   Home"/>
-    <m/>
+    <n v="1"/>
     <x v="1"/>
   </r>
   <r>
@@ -1476,11 +1488,110 @@
     <s v="St. Louis Blues"/>
     <n v="0.47870000000000001"/>
     <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <n v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Colorado Avalanche"/>
+    <n v="0.80030000000000001"/>
+    <s v="San Jose Sharks"/>
+    <n v="0.19969999999999999"/>
+    <s v="Playing At:  Colorado Avalanche   Home"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Edmonton Oilers"/>
+    <n v="0.77249999999999996"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.22750000000000001"/>
+    <s v="Playing At:  Anaheim Ducks   Home"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Dallas Stars"/>
+    <n v="0.68659999999999999"/>
+    <s v="Chicago Blackhawks"/>
+    <n v="0.31340000000000001"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Boston Bruins"/>
+    <n v="0.66520000000000001"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.33479999999999999"/>
+    <s v="Playing At:  Detroit Red Wings   Home"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.60340000000000005"/>
+    <s v="New York Islanders"/>
+    <n v="0.39660000000000001"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Minnesota Wild"/>
+    <n v="0.59240000000000004"/>
+    <s v="Winnipeg Jets"/>
+    <n v="0.40760000000000002"/>
+    <s v="Playing At:  Minnesota Wild   Home"/>
     <m/>
     <x v="1"/>
   </r>
   <r>
     <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Tampa Bay Lightning"/>
+    <n v="0.56240000000000001"/>
+    <s v="Montreal Canadiens"/>
+    <n v="0.43759999999999999"/>
+    <s v="Playing At:  Tampa Bay Lightning   Home"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Ottawa Senators"/>
+    <n v="0.55610000000000004"/>
+    <s v="Buffalo Sabres"/>
+    <n v="0.44390000000000002"/>
+    <s v="Playing At:  Ottawa Senators   Home"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <d v="2023-12-31T00:00:00"/>
+    <s v="Calgary Flames"/>
+    <n v="0.5544"/>
+    <s v="Philadelphia Flyers"/>
+    <n v="0.4456"/>
+    <s v="Playing At:  Calgary Flames   Home"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
     <m/>
     <m/>
     <m/>
@@ -1488,18 +1599,19 @@
     <m/>
     <m/>
     <m/>
-    <x v="2"/>
+    <x v="4"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7A609C84-6A20-4E13-867B-B610F7CD9750}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A3:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" showAll="0">
-      <items count="3">
+      <items count="4">
         <item x="0"/>
+        <item x="2"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -1512,8 +1624,10 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="4">
-        <item h="1" x="2"/>
+      <items count="6">
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
@@ -1524,12 +1638,18 @@
   <rowFields count="1">
     <field x="8"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="5">
     <i>
       <x v="1"/>
     </i>
     <i>
       <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1865,19 +1985,19 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -1885,7 +2005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1902,97 +2022,111 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B4" s="7">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7">
-        <v>14</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="6">
         <f>C4/B4</f>
-        <v>0.58333333333333337</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f>SUM(B4:B6)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <f>SUM(B4:B5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B5" s="7">
-        <v>26</v>
-      </c>
-      <c r="C5" s="7">
-        <v>12</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="6">
         <f t="shared" ref="D5:D9" si="0">C5/B5</f>
-        <v>0.46153846153846156</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f>SUM(C4:C6)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <f>SUM(C4:C5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="7">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6">
         <f>C6/B6</f>
-        <v>0.52</v>
+        <v>0.62962962962962965</v>
       </c>
       <c r="F6" s="6">
         <f>F5/F4</f>
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D7" s="6" t="e">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D8" s="6" t="e">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7">
+        <v>32</v>
+      </c>
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.5423728813559322</v>
       </c>
       <c r="F8">
-        <f>SUM(B7:B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <f>SUM(B6:B7)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F9">
-        <f>SUM(C7:C8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <f>SUM(C6:C7)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
-      <c r="F10" s="6" t="e">
+      <c r="F10" s="6">
         <f>F9/F8</f>
-        <v>#DIV/0!</v>
+        <v>0.56140350877192979</v>
       </c>
     </row>
   </sheetData>
@@ -2002,26 +2136,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -2050,7 +2184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -2080,7 +2214,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -2110,7 +2244,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -2140,7 +2274,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -2170,7 +2304,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -2200,7 +2334,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -2230,7 +2364,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -2260,7 +2394,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2290,7 +2424,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -2320,7 +2454,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -2350,7 +2484,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -2380,7 +2514,7 @@
         <v>80-85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -2410,7 +2544,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -2440,7 +2574,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -2470,7 +2604,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -2500,7 +2634,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -2530,7 +2664,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2560,7 +2694,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2590,7 +2724,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -2620,7 +2754,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2650,7 +2784,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -2680,7 +2814,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2710,7 +2844,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -2740,7 +2874,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2770,7 +2904,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -2800,7 +2934,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2830,7 +2964,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2860,7 +2994,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -2890,7 +3024,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2920,7 +3054,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2950,7 +3084,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -2980,7 +3114,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -3010,7 +3144,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -3040,7 +3174,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -3070,7 +3204,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -3100,7 +3234,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -3130,7 +3264,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -3160,7 +3294,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -3190,7 +3324,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -3220,7 +3354,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -3250,7 +3384,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -3282,7 +3416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -3312,7 +3446,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -3342,7 +3476,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -3372,7 +3506,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3402,7 +3536,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -3432,7 +3566,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -3462,7 +3596,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -3492,7 +3626,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -3522,7 +3656,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -3552,7 +3686,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -3582,7 +3716,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -3612,7 +3746,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -3642,7 +3776,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -3672,7 +3806,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -3702,7 +3836,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -3732,7 +3866,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -3762,7 +3896,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -3792,7 +3926,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -3822,7 +3956,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -3852,7 +3986,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -3882,7 +4016,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -3912,7 +4046,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -3942,7 +4076,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -3972,7 +4106,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -4002,7 +4136,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4032,7 +4166,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -4062,7 +4196,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -4092,7 +4226,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -4122,7 +4256,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -4152,7 +4286,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -4182,7 +4316,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -4212,7 +4346,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -4242,7 +4376,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -4272,7 +4406,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -4302,7 +4436,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -4332,7 +4466,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -4362,7 +4496,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -4392,7 +4526,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -4422,7 +4556,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -4452,7 +4586,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -4482,7 +4616,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -4512,7 +4646,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -4533,13 +4667,16 @@
       </c>
       <c r="G84" t="s">
         <v>50</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
       </c>
       <c r="I84" t="str" cm="1">
         <f t="array" ref="I84">_xlfn.IFS(D84 &gt;= 0.85, "85  &lt;", AND(D84 &gt;=0.8, D84 &lt; 0.85), "80-85", AND(D84 &gt;= 0.7, D84 &lt; 0.8), "70-80", AND(D84 &gt;= 0.6, D84 &lt; 0.7),  "60-70", AND(D84 &gt;= 0.5, D84 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -4560,13 +4697,16 @@
       </c>
       <c r="G85" t="s">
         <v>70</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
       </c>
       <c r="I85" t="str" cm="1">
         <f t="array" ref="I85">_xlfn.IFS(D85 &gt;= 0.85, "85  &lt;", AND(D85 &gt;=0.8, D85 &lt; 0.85), "80-85", AND(D85 &gt;= 0.7, D85 &lt; 0.8), "70-80", AND(D85 &gt;= 0.6, D85 &lt; 0.7),  "60-70", AND(D85 &gt;= 0.5, D85 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -4587,13 +4727,16 @@
       </c>
       <c r="G86" t="s">
         <v>33</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
       </c>
       <c r="I86" t="str" cm="1">
         <f t="array" ref="I86">_xlfn.IFS(D86 &gt;= 0.85, "85  &lt;", AND(D86 &gt;=0.8, D86 &lt; 0.85), "80-85", AND(D86 &gt;= 0.7, D86 &lt; 0.8), "70-80", AND(D86 &gt;= 0.6, D86 &lt; 0.7),  "60-70", AND(D86 &gt;= 0.5, D86 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>82</v>
       </c>
@@ -4614,13 +4757,16 @@
       </c>
       <c r="G87" t="s">
         <v>67</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
       </c>
       <c r="I87" t="str" cm="1">
         <f t="array" ref="I87">_xlfn.IFS(D87 &gt;= 0.85, "85  &lt;", AND(D87 &gt;=0.8, D87 &lt; 0.85), "80-85", AND(D87 &gt;= 0.7, D87 &lt; 0.8), "70-80", AND(D87 &gt;= 0.6, D87 &lt; 0.7),  "60-70", AND(D87 &gt;= 0.5, D87 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -4641,13 +4787,16 @@
       </c>
       <c r="G88" t="s">
         <v>55</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
       </c>
       <c r="I88" t="str" cm="1">
         <f t="array" ref="I88">_xlfn.IFS(D88 &gt;= 0.85, "85  &lt;", AND(D88 &gt;=0.8, D88 &lt; 0.85), "80-85", AND(D88 &gt;= 0.7, D88 &lt; 0.8), "70-80", AND(D88 &gt;= 0.6, D88 &lt; 0.7),  "60-70", AND(D88 &gt;= 0.5, D88 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -4668,13 +4817,16 @@
       </c>
       <c r="G89" t="s">
         <v>48</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
       </c>
       <c r="I89" t="str" cm="1">
         <f t="array" ref="I89">_xlfn.IFS(D89 &gt;= 0.85, "85  &lt;", AND(D89 &gt;=0.8, D89 &lt; 0.85), "80-85", AND(D89 &gt;= 0.7, D89 &lt; 0.8), "70-80", AND(D89 &gt;= 0.6, D89 &lt; 0.7),  "60-70", AND(D89 &gt;= 0.5, D89 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>82</v>
       </c>
@@ -4695,13 +4847,16 @@
       </c>
       <c r="G90" t="s">
         <v>66</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
       </c>
       <c r="I90" t="str" cm="1">
         <f t="array" ref="I90">_xlfn.IFS(D90 &gt;= 0.85, "85  &lt;", AND(D90 &gt;=0.8, D90 &lt; 0.85), "80-85", AND(D90 &gt;= 0.7, D90 &lt; 0.8), "70-80", AND(D90 &gt;= 0.6, D90 &lt; 0.7),  "60-70", AND(D90 &gt;= 0.5, D90 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>82</v>
       </c>
@@ -4722,13 +4877,16 @@
       </c>
       <c r="G91" t="s">
         <v>68</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
       </c>
       <c r="I91" t="str" cm="1">
         <f t="array" ref="I91">_xlfn.IFS(D91 &gt;= 0.85, "85  &lt;", AND(D91 &gt;=0.8, D91 &lt; 0.85), "80-85", AND(D91 &gt;= 0.7, D91 &lt; 0.8), "70-80", AND(D91 &gt;= 0.6, D91 &lt; 0.7),  "60-70", AND(D91 &gt;= 0.5, D91 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>82</v>
       </c>
@@ -4750,8 +4908,254 @@
       <c r="G92" t="s">
         <v>44</v>
       </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
       <c r="I92" t="str" cm="1">
         <f t="array" ref="I92">_xlfn.IFS(D92 &gt;= 0.85, "85  &lt;", AND(D92 &gt;=0.8, D92 &lt; 0.85), "80-85", AND(D92 &gt;= 0.7, D92 &lt; 0.8), "70-80", AND(D92 &gt;= 0.6, D92 &lt; 0.7),  "60-70", AND(D92 &gt;= 0.5, D92 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C93" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="E93" t="s">
+        <v>17</v>
+      </c>
+      <c r="F93" s="2">
+        <v>0.19969999999999999</v>
+      </c>
+      <c r="G93" t="s">
+        <v>18</v>
+      </c>
+      <c r="I93" t="str" cm="1">
+        <f t="array" ref="I93">_xlfn.IFS(D93 &gt;= 0.85, "85  &lt;", AND(D93 &gt;=0.8, D93 &lt; 0.85), "80-85", AND(D93 &gt;= 0.7, D93 &lt; 0.8), "70-80", AND(D93 &gt;= 0.6, D93 &lt; 0.7),  "60-70", AND(D93 &gt;= 0.5, D93 &lt; 0.6), "50-60")</f>
+        <v>80-85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C94" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0.77249999999999996</v>
+      </c>
+      <c r="E94" t="s">
+        <v>23</v>
+      </c>
+      <c r="F94" s="2">
+        <v>0.22750000000000001</v>
+      </c>
+      <c r="G94" t="s">
+        <v>71</v>
+      </c>
+      <c r="I94" t="str" cm="1">
+        <f t="array" ref="I94">_xlfn.IFS(D94 &gt;= 0.85, "85  &lt;", AND(D94 &gt;=0.8, D94 &lt; 0.85), "80-85", AND(D94 &gt;= 0.7, D94 &lt; 0.8), "70-80", AND(D94 &gt;= 0.6, D94 &lt; 0.7),  "60-70", AND(D94 &gt;= 0.5, D94 &lt; 0.6), "50-60")</f>
+        <v>70-80</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>85</v>
+      </c>
+      <c r="B95" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C95" t="s">
+        <v>34</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0.68659999999999999</v>
+      </c>
+      <c r="E95" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0.31340000000000001</v>
+      </c>
+      <c r="G95" t="s">
+        <v>36</v>
+      </c>
+      <c r="I95" t="str" cm="1">
+        <f t="array" ref="I95">_xlfn.IFS(D95 &gt;= 0.85, "85  &lt;", AND(D95 &gt;=0.8, D95 &lt; 0.85), "80-85", AND(D95 &gt;= 0.7, D95 &lt; 0.8), "70-80", AND(D95 &gt;= 0.6, D95 &lt; 0.7),  "60-70", AND(D95 &gt;= 0.5, D95 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C96" t="s">
+        <v>49</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0.66520000000000001</v>
+      </c>
+      <c r="E96" t="s">
+        <v>37</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0.33479999999999999</v>
+      </c>
+      <c r="G96" t="s">
+        <v>38</v>
+      </c>
+      <c r="I96" t="str" cm="1">
+        <f t="array" ref="I96">_xlfn.IFS(D96 &gt;= 0.85, "85  &lt;", AND(D96 &gt;=0.8, D96 &lt; 0.85), "80-85", AND(D96 &gt;= 0.7, D96 &lt; 0.8), "70-80", AND(D96 &gt;= 0.6, D96 &lt; 0.7),  "60-70", AND(D96 &gt;= 0.5, D96 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>85</v>
+      </c>
+      <c r="B97" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C97" t="s">
+        <v>42</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.60340000000000005</v>
+      </c>
+      <c r="E97" t="s">
+        <v>58</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.39660000000000001</v>
+      </c>
+      <c r="G97" t="s">
+        <v>44</v>
+      </c>
+      <c r="I97" t="str" cm="1">
+        <f t="array" ref="I97">_xlfn.IFS(D97 &gt;= 0.85, "85  &lt;", AND(D97 &gt;=0.8, D97 &lt; 0.85), "80-85", AND(D97 &gt;= 0.7, D97 &lt; 0.8), "70-80", AND(D97 &gt;= 0.6, D97 &lt; 0.7),  "60-70", AND(D97 &gt;= 0.5, D97 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>85</v>
+      </c>
+      <c r="B98" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C98" t="s">
+        <v>43</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.59240000000000004</v>
+      </c>
+      <c r="E98" t="s">
+        <v>31</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.40760000000000002</v>
+      </c>
+      <c r="G98" t="s">
+        <v>69</v>
+      </c>
+      <c r="I98" t="str" cm="1">
+        <f t="array" ref="I98">_xlfn.IFS(D98 &gt;= 0.85, "85  &lt;", AND(D98 &gt;=0.8, D98 &lt; 0.85), "80-85", AND(D98 &gt;= 0.7, D98 &lt; 0.8), "70-80", AND(D98 &gt;= 0.6, D98 &lt; 0.7),  "60-70", AND(D98 &gt;= 0.5, D98 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C99" t="s">
+        <v>46</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.56240000000000001</v>
+      </c>
+      <c r="E99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.43759999999999999</v>
+      </c>
+      <c r="G99" t="s">
+        <v>48</v>
+      </c>
+      <c r="I99" t="str" cm="1">
+        <f t="array" ref="I99">_xlfn.IFS(D99 &gt;= 0.85, "85  &lt;", AND(D99 &gt;=0.8, D99 &lt; 0.85), "80-85", AND(D99 &gt;= 0.7, D99 &lt; 0.8), "70-80", AND(D99 &gt;= 0.6, D99 &lt; 0.7),  "60-70", AND(D99 &gt;= 0.5, D99 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>85</v>
+      </c>
+      <c r="B100" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C100" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.55610000000000004</v>
+      </c>
+      <c r="E100" t="s">
+        <v>53</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0.44390000000000002</v>
+      </c>
+      <c r="G100" t="s">
+        <v>78</v>
+      </c>
+      <c r="I100" t="str" cm="1">
+        <f t="array" ref="I100">_xlfn.IFS(D100 &gt;= 0.85, "85  &lt;", AND(D100 &gt;=0.8, D100 &lt; 0.85), "80-85", AND(D100 &gt;= 0.7, D100 &lt; 0.8), "70-80", AND(D100 &gt;= 0.6, D100 &lt; 0.7),  "60-70", AND(D100 &gt;= 0.5, D100 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>85</v>
+      </c>
+      <c r="B101" s="1">
+        <v>45291</v>
+      </c>
+      <c r="C101" t="s">
+        <v>40</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.5544</v>
+      </c>
+      <c r="E101" t="s">
+        <v>56</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0.4456</v>
+      </c>
+      <c r="G101" t="s">
+        <v>41</v>
+      </c>
+      <c r="I101" t="str" cm="1">
+        <f t="array" ref="I101">_xlfn.IFS(D101 &gt;= 0.85, "85  &lt;", AND(D101 &gt;=0.8, D101 &lt; 0.85), "80-85", AND(D101 &gt;= 0.7, D101 &lt; 0.8), "70-80", AND(D101 &gt;= 0.6, D101 &lt; 0.7),  "60-70", AND(D101 &gt;= 0.5, D101 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>

</xml_diff>